<commit_message>
Find definitions of acronyms. Pyramid charts. Split single .Rmd file into several smaller ones
</commit_message>
<xml_diff>
--- a/CRR Custom Words.xlsx
+++ b/CRR Custom Words.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hot_words" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>bribery</t>
   </si>
@@ -137,6 +137,27 @@
   </si>
   <si>
     <t>greenhouse</t>
+  </si>
+  <si>
+    <t>www</t>
+  </si>
+  <si>
+    <t>ag</t>
+  </si>
+  <si>
+    <t>chf</t>
+  </si>
+  <si>
+    <t>usd</t>
+  </si>
+  <si>
+    <t>gbp</t>
+  </si>
+  <si>
+    <t>jpy</t>
+  </si>
+  <si>
+    <t>eur</t>
   </si>
 </sst>
 </file>
@@ -499,7 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -675,9 +696,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -734,6 +757,41 @@
         <v>2016</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>